<commit_message>
Hoan thien tinh nang FaceID va Fix loi API
</commit_message>
<xml_diff>
--- a/KHCN_QR_List-KHCN.xlsx
+++ b/KHCN_QR_List-KHCN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\khcn-attendance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{716E1A48-0F7A-41DB-94C7-5B76E46AB3E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2313E6A-8D8B-45C6-99DF-7532F2C58587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -602,7 +602,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>